<commit_message>
Aging Rack Setting 정보 표시
</commit_message>
<xml_diff>
--- a/FMSMonitoringUI/TagList/TAGS_CLIENT_V1.xlsx
+++ b/FMSMonitoringUI/TagList/TAGS_CLIENT_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0000.GIT\FMSMonitoringUI\FMSMonitoringUI\TagList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B808E07-5757-480C-BE9A-A74171ED0DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081F72E4-77F8-499C-AEBC-77683592D8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{66441DF0-A1AE-4821-9768-E7E31D0D2B1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{66441DF0-A1AE-4821-9768-E7E31D0D2B1A}"/>
   </bookViews>
   <sheets>
     <sheet name="EQPLIST" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="96">
   <si>
     <t>Type</t>
   </si>
@@ -400,6 +400,12 @@
   <si>
     <t>Equipment ID는 Code에서 생성하여 Tag List생성</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FMSTrouble</t>
+  </si>
+  <si>
+    <t>MachineTrouble</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1548,7 @@
   <dimension ref="B1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1694,7 +1700,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>18</v>
@@ -1711,7 +1717,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>21</v>
@@ -1725,7 +1731,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>21</v>
@@ -1750,7 +1756,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>24</v>
@@ -1767,7 +1773,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>17</v>
@@ -1781,7 +1787,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>21</v>
@@ -2543,6 +2549,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101002F4D9E66E572D64B89A6A9DAE4986E6C" ma:contentTypeVersion="10" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="1c573c41012530a44f06d88224461ca6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="86689cf0-44ed-43c5-8873-dd032250b33c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c1fb380cb2ac8836ad9eed3cdcc8d48" ns3:_="">
     <xsd:import namespace="86689cf0-44ed-43c5-8873-dd032250b33c"/>
@@ -2726,22 +2747,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5945D743-C37D-43A2-8DD9-4C38CE1B673B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1117DF4-1F58-48DF-B1E3-B2D5FF9228BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="86689cf0-44ed-43c5-8873-dd032250b33c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42BA27C-AA71-401C-8049-F1FF9447B7D4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2757,28 +2787,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5945D743-C37D-43A2-8DD9-4C38CE1B673B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1117DF4-1F58-48DF-B1E3-B2D5FF9228BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="86689cf0-44ed-43c5-8873-dd032250b33c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Conveyor Rework Tray Check
</commit_message>
<xml_diff>
--- a/FMSMonitoringUI/TagList/TAGS_CLIENT_V1.xlsx
+++ b/FMSMonitoringUI/TagList/TAGS_CLIENT_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0000.GIT\FMSMonitoringUI\FMSMonitoringUI\TagList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9906EE61-AFB6-4495-B6BA-67B7C5CA8657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E48103-BD3C-4458-8B80-12C2E6BEF33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66441DF0-A1AE-4821-9768-E7E31D0D2B1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{66441DF0-A1AE-4821-9768-E7E31D0D2B1A}"/>
   </bookViews>
   <sheets>
     <sheet name="EQPLIST" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="93">
   <si>
     <t>Type</t>
   </si>
@@ -230,18 +230,6 @@
   </si>
   <si>
     <t>Comments</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MethodArgInOut</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Historize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BatchReport</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1035,10 +1023,10 @@
         <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -1046,10 +1034,10 @@
         <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1063,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB43E730-868F-430D-BD24-ADD2940A8B70}">
   <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1114,7 +1102,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
@@ -1124,7 +1112,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -1132,7 +1120,7 @@
         <v>35</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>13</v>
@@ -1222,7 +1210,9 @@
         <v>21</v>
       </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
@@ -1545,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C811ADC-063A-4F19-91CF-5DFCB74A36A9}">
   <dimension ref="B1:H70"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1555,7 +1545,7 @@
     <col min="2" max="2" width="22.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="37" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.25" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="89" style="1" customWidth="1"/>
@@ -1587,19 +1577,19 @@
       <c r="D3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>52</v>
+      <c r="E3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
@@ -1609,7 +1599,7 @@
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -1617,7 +1607,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>13</v>
@@ -1645,7 +1635,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>13</v>
@@ -1693,12 +1683,14 @@
         <v>21</v>
       </c>
       <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>18</v>
@@ -1715,7 +1707,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>21</v>
@@ -1729,7 +1721,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>21</v>
@@ -1743,7 +1735,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>13</v>
@@ -1754,7 +1746,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>24</v>
@@ -1771,7 +1763,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>17</v>
@@ -1785,7 +1777,7 @@
         <v>10</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>21</v>
@@ -1810,10 +1802,10 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>13</v>
@@ -1824,10 +1816,10 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>13</v>
@@ -1838,24 +1830,26 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="F21" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>21</v>
@@ -1866,10 +1860,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>17</v>
@@ -1880,10 +1874,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>13</v>
@@ -1894,10 +1888,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>17</v>
@@ -1908,10 +1902,10 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>17</v>
@@ -1922,10 +1916,10 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>21</v>
@@ -1939,21 +1933,23 @@
         <v>12</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
+      <c r="F28" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="G28" s="9"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>17</v>
@@ -1964,10 +1960,10 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>17</v>
@@ -1978,10 +1974,10 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>17</v>
@@ -1992,10 +1988,10 @@
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>17</v>
@@ -2006,10 +2002,10 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>17</v>
@@ -2020,10 +2016,10 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>17</v>
@@ -2034,10 +2030,10 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>17</v>
@@ -2048,10 +2044,10 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>17</v>
@@ -2062,10 +2058,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>21</v>
@@ -2079,7 +2075,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>31</v>
@@ -2093,7 +2089,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>31</v>
@@ -2107,7 +2103,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>21</v>
@@ -2118,10 +2114,10 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>13</v>
@@ -2132,10 +2128,10 @@
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>21</v>
@@ -2146,10 +2142,10 @@
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>21</v>
@@ -2160,10 +2156,10 @@
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>21</v>
@@ -2174,10 +2170,10 @@
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>21</v>
@@ -2188,10 +2184,10 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>21</v>
@@ -2202,10 +2198,10 @@
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>17</v>
@@ -2216,10 +2212,10 @@
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>13</v>
@@ -2230,10 +2226,10 @@
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>21</v>
@@ -2244,10 +2240,10 @@
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>21</v>
@@ -2258,10 +2254,10 @@
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>21</v>
@@ -2272,10 +2268,10 @@
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>21</v>
@@ -2286,10 +2282,10 @@
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>21</v>
@@ -2300,10 +2296,10 @@
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>17</v>
@@ -2314,10 +2310,10 @@
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>13</v>
@@ -2331,7 +2327,7 @@
         <v>20</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>21</v>
@@ -2342,10 +2338,10 @@
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>17</v>
@@ -2359,7 +2355,7 @@
         <v>12</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>17</v>
@@ -2375,7 +2371,7 @@
         <v>41</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>31</v>
@@ -2389,7 +2385,7 @@
         <v>42</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>31</v>
@@ -2403,7 +2399,7 @@
         <v>40</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>21</v>
@@ -2414,10 +2410,10 @@
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D62" s="11" t="s">
         <v>13</v>
@@ -2428,10 +2424,10 @@
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>21</v>
@@ -2442,10 +2438,10 @@
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>21</v>
@@ -2456,10 +2452,10 @@
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>21</v>
@@ -2470,10 +2466,10 @@
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>21</v>
@@ -2484,10 +2480,10 @@
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>21</v>
@@ -2498,10 +2494,10 @@
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>17</v>
@@ -2512,10 +2508,10 @@
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>17</v>
@@ -2526,10 +2522,10 @@
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>17</v>
@@ -2545,12 +2541,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101002F4D9E66E572D64B89A6A9DAE4986E6C" ma:contentTypeVersion="10" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="1c573c41012530a44f06d88224461ca6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="86689cf0-44ed-43c5-8873-dd032250b33c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c1fb380cb2ac8836ad9eed3cdcc8d48" ns3:_="">
     <xsd:import namespace="86689cf0-44ed-43c5-8873-dd032250b33c"/>
@@ -2734,16 +2739,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5945D743-C37D-43A2-8DD9-4C38CE1B673B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1117DF4-1F58-48DF-B1E3-B2D5FF9228BE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2759,7 +2763,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42BA27C-AA71-401C-8049-F1FF9447B7D4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2775,12 +2779,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5945D743-C37D-43A2-8DD9-4C38CE1B673B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ver.2023.05.04.001 Aging Remark 기능추가
</commit_message>
<xml_diff>
--- a/FMSMonitoringUI/TagList/TAGS_CLIENT_V1.xlsx
+++ b/FMSMonitoringUI/TagList/TAGS_CLIENT_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0000.GIT\FMSMonitoringUI\FMSMonitoringUI\TagList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7359DD37-52FF-4201-B500-CC36C5238498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35D738C-8199-42D6-B8D3-E604A5DA7333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66441DF0-A1AE-4821-9768-E7E31D0D2B1A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66441DF0-A1AE-4821-9768-E7E31D0D2B1A}"/>
   </bookViews>
   <sheets>
     <sheet name="EQPLIST" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="97">
   <si>
     <t>Type</t>
   </si>
@@ -408,6 +408,10 @@
   </si>
   <si>
     <t>WaterTank2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrorLevel</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1078,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB43E730-868F-430D-BD24-ADD2940A8B70}">
   <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1289,7 +1293,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>10</v>
+        <v>96</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>22</v>
@@ -2787,21 +2791,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101002F4D9E66E572D64B89A6A9DAE4986E6C" ma:contentTypeVersion="10" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="1c573c41012530a44f06d88224461ca6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="86689cf0-44ed-43c5-8873-dd032250b33c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c1fb380cb2ac8836ad9eed3cdcc8d48" ns3:_="">
     <xsd:import namespace="86689cf0-44ed-43c5-8873-dd032250b33c"/>
@@ -2985,10 +2974,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5945D743-C37D-43A2-8DD9-4C38CE1B673B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42BA27C-AA71-401C-8049-F1FF9447B7D4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="86689cf0-44ed-43c5-8873-dd032250b33c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3010,19 +3024,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42BA27C-AA71-401C-8049-F1FF9447B7D4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5945D743-C37D-43A2-8DD9-4C38CE1B673B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="86689cf0-44ed-43c5-8873-dd032250b33c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>